<commit_message>
refactor creating seeds from exel file
</commit_message>
<xml_diff>
--- a/app/services/seed_generator/Seeds.xlsx
+++ b/app/services/seed_generator/Seeds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
   <si>
     <t>name</t>
   </si>
@@ -28,7 +28,7 @@
     <t>picture_path</t>
   </si>
   <si>
-    <t>product_cathegory</t>
+    <t>product_cathegory_id</t>
   </si>
   <si>
     <t>promoted_from</t>
@@ -82,6 +82,9 @@
     <t>https://olx-development.s3.eu-central-1.amazonaws.com/images/products/constuction_chemicals/tynk+akrylowy.jpeg</t>
   </si>
   <si>
+    <t>2022-10-27 13:18:43.685298</t>
+  </si>
+  <si>
     <t>Tynk mozaikowy</t>
   </si>
   <si>
@@ -308,6 +311,9 @@
   </si>
   <si>
     <t>1234Hbjkadasd</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
   <si>
     <t>1234Hbjkajjkkaasd</t>
@@ -604,6 +610,8 @@
     <col customWidth="1" min="3" max="3" width="15.0"/>
     <col customWidth="1" min="4" max="4" width="24.5"/>
     <col customWidth="1" min="5" max="5" width="18.38"/>
+    <col customWidth="1" min="6" max="6" width="23.5"/>
+    <col customWidth="1" min="7" max="7" width="23.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -713,19 +721,25 @@
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>10.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -733,16 +747,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>10.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
@@ -750,325 +764,328 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>1000.0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>46.0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1">
         <v>12.0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>50.0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1">
         <v>50.0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1">
         <v>50.0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1">
         <v>100.0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1">
         <v>100.0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1">
         <v>100.0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1">
         <v>30.0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1">
         <v>125.0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1">
         <v>80.0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1">
         <v>24.0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1">
         <v>12.0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1">
         <v>50.0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1">
         <v>20.0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1">
         <v>130.0</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="1">
         <v>15.0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1">
         <v>45.0</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1138,6 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -1130,22 +1146,22 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1169,35 +1185,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <v>5.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1">
         <v>4.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1221,29 +1237,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>